<commit_message>
User checkpoint: No changes made to CNBS Business Bank Statement.
</commit_message>
<xml_diff>
--- a/attached_assets/CNBS Business Bank Statement.xlsx
+++ b/attached_assets/CNBS Business Bank Statement.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Festu\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1B75C4-8BCF-414C-AA89-9AE5D1767F74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C33D33E-1DF5-4896-87A1-9AF4A9F4227F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1283,7 +1283,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="8" formatCode="&quot;R&quot;#,##0.00;[Red]\-&quot;R&quot;#,##0.00"/>
-    <numFmt numFmtId="164" formatCode="yyyy/mm/dd;@"/>
+    <numFmt numFmtId="167" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -1349,10 +1349,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1662,12 +1662,12 @@
   <dimension ref="A1:C881"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" style="6" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="51.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.140625" style="4" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>